<commit_message>
remove sy-datum/sy-uzeit from demo programs
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel1.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel1.w3mi.data.xlsx
@@ -419,10 +419,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="2">
-        <v>44557</v>
+        <v>44561</v>
       </c>
       <c r="C3" s="3">
-        <v>0.7721990740740741</v>
+        <v>0.2488078703703704</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>